<commit_message>
Added output file for 321 priority
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:W9"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -503,7 +503,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -583,13 +583,32 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -606,25 +625,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added c file for 213 priority , output files for 312 priority
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="R7" sqref="R7:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -498,7 +498,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -590,25 +590,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -625,6 +606,25 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added c file for 231 priority and output file for 213 priority
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7:T7"/>
+      <selection activeCell="L9" sqref="L9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -488,7 +488,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -568,7 +568,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -590,6 +590,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -606,25 +625,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added output files for 231 scheduling , modified c file for 123 scheduling
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:N9"/>
+      <selection activeCell="O7" sqref="O7:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -493,7 +493,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -590,25 +590,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -625,6 +606,25 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added output files for 123 priority , changed c file for 132 priority
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:Q7"/>
+      <selection activeCell="F9" sqref="F9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -478,7 +478,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -558,7 +558,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -590,6 +590,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -606,25 +625,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added results for 132 priority
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="B5:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H9"/>
+      <selection activeCell="I7" sqref="I7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -483,7 +483,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -590,25 +590,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="U9:W9"/>
@@ -625,6 +606,25 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>